<commit_message>
Aize QA Assignment Final Commit
</commit_message>
<xml_diff>
--- a/Task1 Manual TestCase/TestCases for Swag Labs Application.xlsx
+++ b/Task1 Manual TestCase/TestCases for Swag Labs Application.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vardha_P\Aize\Task1 Manual TestCase\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB825F0-C467-4D51-B387-2492FE8A7CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{61732CB6-C3D7-445F-A02A-7E4400CFDE7C}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -593,9 +587,6 @@
     <t>The URL's of checkout : you information page and Checkout: Overview page should match.</t>
   </si>
   <si>
-    <t>The payment information should have unique SauceCard ID number.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Step iv) Check if the payment information has unique SauceCard ID number. i.e, </t>
     </r>
@@ -706,9 +697,6 @@
   </si>
   <si>
     <t>User should not be allowed to checkout because there is not items in cart.</t>
-  </si>
-  <si>
-    <t>Steps iii) Check if the user can checkout</t>
   </si>
   <si>
     <t>user should be able to login swag labs successfully.</t>
@@ -835,11 +823,17 @@
   <si>
     <t>The application should not navigate to login screen and it should go back to the previous history or new tab if no history is available. (Single page apps concept)</t>
   </si>
+  <si>
+    <t>The payment information should have unique SauceCard #ID number.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps iii) Check if the user can checkout and place the order. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -897,7 +891,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -919,6 +913,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE7E7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1040,12 +1040,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE7E7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1100,7 +1111,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1152,7 +1163,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1346,28 +1357,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4224EC-3609-4105-9BB8-343A25F5E3D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="78.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="61" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1384,21 +1395,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -1408,7 +1419,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -1418,7 +1429,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -1438,7 +1449,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1448,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1462,7 +1473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -1472,7 +1483,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
@@ -1482,7 +1493,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -1492,7 +1503,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1506,7 +1517,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2" t="s">
@@ -1516,7 +1527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="2" t="s">
@@ -1526,7 +1537,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="29.45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="4" t="s">
@@ -1536,7 +1547,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1550,7 +1561,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
@@ -1560,7 +1571,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
@@ -1570,37 +1581,37 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D19" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29.45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -1611,256 +1622,256 @@
         <v>33</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="C35" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>